<commit_message>
feat: more transfer logic
</commit_message>
<xml_diff>
--- a/pkg/parser/testdata/currency_exchange.xlsx
+++ b/pkg/parser/testdata/currency_exchange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\iqpirat\sources\github\firefly-iii-privatbank-importer\pkg\parser\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ADC9D6-AA0C-4397-B35F-C01A0983822B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F550B6-CD6E-4342-B99B-ADF9DDAB8590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="3240" windowWidth="28800" windowHeight="15345" xr2:uid="{59FE2EEA-6F4F-4CBD-B376-F495B0D7EFC1}"/>
+    <workbookView xWindow="-1935" yWindow="4350" windowWidth="28800" windowHeight="15345" xr2:uid="{59FE2EEA-6F4F-4CBD-B376-F495B0D7EFC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>